<commit_message>
Adding updated worksheets with algorithm that reflects all scenarios, and pass fail criteria.
</commit_message>
<xml_diff>
--- a/worksheets/Accessibility Page Score - Electronic Content.xlsx
+++ b/worksheets/Accessibility Page Score - Electronic Content.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>CONSTANT VALUES - Do Not Modify</t>
   </si>
@@ -31,6 +31,11 @@
     <t>ERROR MULTIPLIERS - Values Will Change Based on Yes/No Answers Below</t>
   </si>
   <si>
+    <t>Calculated values for
+manual error multplier.
+Do not modify.</t>
+  </si>
+  <si>
     <t>Screenreader error multiplier</t>
   </si>
   <si>
@@ -65,6 +70,11 @@
   </si>
   <si>
     <t>AUTOMATED TEST ERRORS - Update These Values</t>
+  </si>
+  <si>
+    <t>Calculated values for
+errors by axe category.
+Do not modify.</t>
   </si>
   <si>
     <t>No. of critical axe-core errors</t>
@@ -117,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="mmm d, yyyy"/>
     <numFmt numFmtId="165" formatCode="mmm&quot; &quot;d&quot;, &quot;yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -135,6 +145,10 @@
     <font/>
     <font>
       <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -147,7 +161,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,14 +176,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -198,16 +218,26 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -216,13 +246,16 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -240,7 +273,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -275,6 +308,18 @@
       </fill>
       <border/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
   </dxfs>
 </styleSheet>
 </file>
@@ -291,7 +336,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="64.43"/>
-    <col customWidth="1" min="2" max="2" width="28.71"/>
+    <col customWidth="1" min="2" max="3" width="28.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.75" customHeight="1">
@@ -361,226 +406,298 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="37.5">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
-        <f>IF(B27 = "Yes", 1.03, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5">
-        <f>IF(B28 = "Yes", 1.125, 1)</f>
+        <f>IF(B29 = "Yes", 1.03, 1)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="9">
+        <f>IF(B9=1, 0, B9 + 1/(B9/B17))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5">
-        <f>IF(B29 = "Yes", 1.08, 1)</f>
+        <f>IF(B30 = "Yes", 1.125, 1)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="9">
+        <f>IF(B10=1, 0, B10 + 1/(B10/B17))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5">
-        <f>IF(B30 = "Yes", 1.03, 1)</f>
+        <f>IF(B31 = "Yes", 1.08, 1)</f>
         <v>1</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="13" ht="27.75" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="C11" s="9">
+        <f>IF(B11=1, 0, B11 + 1/(B11/B17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="B12" s="5">
+        <f>IF(B32 = "Yes", 1.03, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <f>IF(B12=1, 0, B12 + 1/(B12/B17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" ht="27.75" customHeight="1">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="10">
-        <v>0.0</v>
-      </c>
+      <c r="B16" s="15"/>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>15</v>
+      <c r="B17" s="14">
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" ht="27.75" customHeight="1">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="B19" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" ht="27.75" customHeight="1">
+      <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="13" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+    </row>
+    <row r="22" ht="37.5">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5">
-        <v>0.0</v>
-      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="5">
         <v>0.0</v>
       </c>
+      <c r="C23">
+        <f>B23 * 4</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C24">
+        <f>B24 * 3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C25">
+        <f>B25 * 2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="5">
         <v>3.0</v>
       </c>
-    </row>
-    <row r="26" ht="27.75" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="C26">
+        <f>B26</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" ht="27.75" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="30">
@@ -588,71 +705,87 @@
         <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" ht="27.75" customHeight="1">
-      <c r="A32" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="14" t="s">
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="15">
-        <f>IF(B16 = 0, 0, ((SUM(4*B21, 3*B22, 2*B23, B24)) * (B8 * B9 * B10 * B11))/B16)</f>
-        <v>0</v>
-      </c>
-      <c r="C33" s="16" t="str">
-        <f>B15</f>
+      <c r="B32" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" ht="27.75" customHeight="1">
+      <c r="A34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="13"/>
+      <c r="Y34" s="13"/>
+      <c r="Z34" s="13"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="20">
+        <f>IF(AND(B17&gt;= 1,B23=0,B24=0,B25=0,B26=0,B29="No",B30="No",B31="No",B32="No"), 0, (IF(AND(B23=0,B24=0,B25=0,B26=0), ((SUM(C9, C10, C11, C12) * B18) / B18), (SUM(SUM(C23, C24, C25, C26), SUM(C9, C10, C11, C12) * B17)) / B17)))</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="21" t="str">
+        <f>B16</f>
         <v/>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="17" t="str">
+    <row r="36">
+      <c r="A36" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="22" t="str">
+        <f>B19</f>
+        <v>n/a</v>
+      </c>
+      <c r="C36" s="23" t="str">
         <f>B18</f>
         <v>n/a</v>
       </c>
-      <c r="C34" s="18" t="str">
-        <f>B17</f>
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="19">
-        <f>IF(B18 = "n/a", 0, ((B33 - B34)/B34))</f>
+    </row>
+    <row r="37">
+      <c r="A37" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="24">
+        <f>IF(B19 = "n/a", 0, ((B35 - B36)/B36))</f>
         <v>0</v>
       </c>
     </row>
@@ -660,26 +793,31 @@
   <mergeCells count="1">
     <mergeCell ref="A7:Z7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B35">
+  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>"0%"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
+  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>"0%"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
+  <conditionalFormatting sqref="B37">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"0%"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B27">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B29">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B28:B30">
+    <dataValidation type="list" allowBlank="1" sqref="B30:B32">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>